<commit_message>
add updated observed 1st import data
</commit_message>
<xml_diff>
--- a/data/mpox_Asia_importation_date.xlsx
+++ b/data/mpox_Asia_importation_date.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aflub\Desktop\prj_LSHTM_study\prj_project_mpox_in_Asia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473D675D-41B5-48F9-A8A1-0BB7C336369E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BC1ED3-A09A-4BF7-91C2-992336479795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="707" yWindow="707" windowWidth="19200" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15300" yWindow="5445" windowWidth="14445" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Country</t>
     <phoneticPr fontId="1"/>
@@ -328,13 +328,31 @@
   <si>
     <t>SAU</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2024-12-15</t>
+  </si>
+  <si>
+    <t>2024-09-01</t>
+  </si>
+  <si>
+    <t>2023-01-11</t>
+  </si>
+  <si>
+    <t>ARE</t>
+  </si>
+  <si>
+    <t>JOR</t>
+  </si>
+  <si>
+    <t>CYP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -598,18 +616,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A8F522-1FF1-4BFA-992A-532DCCC13C92}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.7"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1171875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +647,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -646,7 +664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -663,7 +681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -680,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -697,7 +715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -714,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -731,7 +749,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -745,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -759,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -776,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -790,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -804,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -818,7 +836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -832,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -846,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -863,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -877,12 +895,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -896,7 +914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -910,32 +928,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -949,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -963,7 +1008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>